<commit_message>
added consumption summary at end of August
</commit_message>
<xml_diff>
--- a/GOM_GuessOMeter/guessometer.xlsx
+++ b/GOM_GuessOMeter/guessometer.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwesTechnik\Ioniq28Investigations\GOM_GuessOMeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AD492D-E15C-4161-A6B0-7D84CDC7C81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E9B240-C27F-49FB-B7F0-7DE1684FA66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="0" windowWidth="20295" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="20295" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="historyJune2025" sheetId="1" r:id="rId1"/>
+    <sheet name="historyAugust2025" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>km</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>estimated range (with 23kWh)</t>
+  </si>
+  <si>
+    <t>Conclusion: good match</t>
   </si>
 </sst>
 </file>
@@ -385,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,4 +916,534 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50573623-EB5B-4FFE-9E6F-1C77146736EF}">
+  <dimension ref="A5:L44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>11.7</v>
+      </c>
+      <c r="E6">
+        <f>D6/100*C6</f>
+        <v>0.81899999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>794</v>
+      </c>
+      <c r="D7">
+        <v>11.7</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E35" si="0">D7/100*C7</f>
+        <v>92.897999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>10.1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>6.5649999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>9.4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>6.2039999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>10.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4.7520000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>8.6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3.2679999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>6.1740000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>10.4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6.8640000000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>266</v>
+      </c>
+      <c r="D14">
+        <v>11.4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>30.324000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>81</v>
+      </c>
+      <c r="D15">
+        <v>10.4</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>8.4240000000000013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>672</v>
+      </c>
+      <c r="D16">
+        <v>11.8</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>79.296000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>973</v>
+      </c>
+      <c r="D17">
+        <v>13.4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>130.38200000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>2136</v>
+      </c>
+      <c r="D18">
+        <v>11.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>245.64000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>84</v>
+      </c>
+      <c r="D19">
+        <v>11.1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>9.3239999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>1534</v>
+      </c>
+      <c r="D20">
+        <v>11.9</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>182.54600000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>1088</v>
+      </c>
+      <c r="D21">
+        <v>13.7</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>149.05599999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>1066</v>
+      </c>
+      <c r="D22">
+        <v>13.6</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>144.976</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>13.6</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.95200000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>359</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>43.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>58</v>
+      </c>
+      <c r="D25">
+        <v>9.6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>5.5680000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>296</v>
+      </c>
+      <c r="D26">
+        <v>12.8</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>37.887999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>79</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>12.7</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2.1589999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>12.2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.952</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>79</v>
+      </c>
+      <c r="D30">
+        <v>11.8</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>9.322000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>196</v>
+      </c>
+      <c r="D31">
+        <v>11.8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>23.128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.77599999999999991</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>15.5</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>40</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>12.6</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f>SUM(C6:C35)</f>
+        <v>10207</v>
+      </c>
+      <c r="E37">
+        <f>SUM(E6:E35)</f>
+        <v>1247.867</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <f>E37*100/C37</f>
+        <v>12.225600078377584</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <f>28/D39*100</f>
+        <v>229.0276127183426</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="L41">
+        <f>23/D39*100</f>
+        <v>188.12982473292428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>